<commit_message>
first realse with api
</commit_message>
<xml_diff>
--- a/temp_data/temp_gcn/csv/temp.xlsx
+++ b/temp_data/temp_gcn/csv/temp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>xmin</t>
   </si>
@@ -34,109 +34,235 @@
     <t>labels</t>
   </si>
   <si>
-    <t>Phụ lục 3</t>
-  </si>
-  <si>
-    <t>Ngày 19 2022</t>
-  </si>
-  <si>
-    <t>SỞ Y TẾ</t>
-  </si>
-  <si>
-    <t>TỈNH ĐIỆN BIÊN</t>
-  </si>
-  <si>
-    <t>CỘNG HÒA XÃ HỘI CHỦ NGHĨA VIỆT NAM</t>
-  </si>
-  <si>
-    <t>MS: 01/BV-01</t>
-  </si>
-  <si>
-    <t>TRUNG TÂM Y TẾ HUYỆN</t>
-  </si>
-  <si>
-    <t>Độc lập - Tự do - Hạnh phúc</t>
-  </si>
-  <si>
-    <t>Số lưu trữ:</t>
-  </si>
-  <si>
-    <t>MƯỜNG ẢNG</t>
-  </si>
-  <si>
-    <t>Mã y tế: 1108222001631</t>
-  </si>
-  <si>
-    <t>Khoa Y học cổ truyền: Khoa chỉ thái</t>
-  </si>
-  <si>
-    <t>Vật lý trị liệu - Phục hồi chức</t>
+    <t>polygon</t>
+  </si>
+  <si>
+    <t>CỘNG HÒA XÃ HỘI CHỦ NGHĨA VIỆT NAM MS: 01/BV-01</t>
+  </si>
+  <si>
+    <t>SỞ Y TẾ THÁI NGUYÊN</t>
+  </si>
+  <si>
+    <t>BV ĐK YÊN BÌNH THÁI NGUYÊN</t>
+  </si>
+  <si>
+    <t>Số lưu trữ: 22KNG -001740</t>
+  </si>
+  <si>
+    <t>Độc lập- Tự do- Hạnh phúc</t>
+  </si>
+  <si>
+    <t>Khoa ngoại tổng hợp</t>
+  </si>
+  <si>
+    <t>Mã y tế: 40113322009003</t>
   </si>
   <si>
     <t>GIẤY RA VIỆN</t>
   </si>
   <si>
-    <t>Họ tên người bệnh: VŨ THỊ PHƯƠNG</t>
-  </si>
-  <si>
-    <t>Tuổi: 39 Nam/Nữ: Nữ</t>
-  </si>
-  <si>
-    <t>Dân tộc: Kinh</t>
-  </si>
-  <si>
-    <t>Nghề Nghiệp: Công nhân viên</t>
-  </si>
-  <si>
-    <t>Mã số BHXH: 0110150920</t>
-  </si>
-  <si>
-    <t>Mã thẻ BHYT: DN 4 11 0110150920</t>
-  </si>
-  <si>
-    <t>Địa chỉ: Tổ 4, Thị trấn Mường Ảng, Huyện Mường Ảng, Tỉnh Điện Biên</t>
-  </si>
-  <si>
-    <t>Vào viện lúc: 07 Giờ 48 Phút, Ngày 28 tháng 12 năm 2021</t>
-  </si>
-  <si>
-    <t>08 Giờ 00 Phút, Ngày 11 tháng 01 năm 2022</t>
-  </si>
-  <si>
-    <t>Ra viện lúc:</t>
-  </si>
-  <si>
-    <t>Chẩn đoán: đau dây thần kinh tọa hai bên / rối loạn tuần hoàn não</t>
-  </si>
-  <si>
-    <t>thể trạng ,điện châm , xoa</t>
-  </si>
-  <si>
-    <t>Phương pháp điều trị: tăng tuần hoàn não ,giảm đau ,nâng cao</t>
-  </si>
-  <si>
-    <t>bóp vùng,chiếu đèn hồng ngoại</t>
-  </si>
-  <si>
-    <t>Ghi Chú:</t>
-  </si>
-  <si>
-    <t>Ngày 11 tháng 01 năm 2022</t>
-  </si>
-  <si>
-    <t>TRƯỞNG KHOA</t>
-  </si>
-  <si>
-    <t>THỦ TRƯƠNG ĐƠN VỊ</t>
-  </si>
-  <si>
-    <t>Cà Thị Hòa</t>
-  </si>
-  <si>
-    <t>BSCKT. Bài Thanh Mai</t>
+    <t>Nữ</t>
+  </si>
+  <si>
+    <t>- Họ tên người bệnh: QUÁCH THỊ THU</t>
+  </si>
+  <si>
+    <t>Tuổi: 27 tuổi</t>
+  </si>
+  <si>
+    <t>- Dân tộc:</t>
+  </si>
+  <si>
+    <t>Mường</t>
+  </si>
+  <si>
+    <t>Nghề nghiệp: Công nhân</t>
+  </si>
+  <si>
+    <t>- Mã số BHXH/Thẻ BHYT số:</t>
+  </si>
+  <si>
+    <t>DN 4 19 19 14817758</t>
+  </si>
+  <si>
+    <t>- Địa chỉ:</t>
+  </si>
+  <si>
+    <t>Phượng Nghi, Như Thanh, Thanh Hóa</t>
+  </si>
+  <si>
+    <t>- Vào viện lúc:</t>
+  </si>
+  <si>
+    <t>08 giờ 52 phút ngày 26 tháng 09 năm 2022</t>
+  </si>
+  <si>
+    <t>- Ra viện lúc:</t>
+  </si>
+  <si>
+    <t>15 giờ 00 phút ngày 06 tháng 10 năm 2022</t>
+  </si>
+  <si>
+    <t>- Chẩn đoán:</t>
+  </si>
+  <si>
+    <t>S06.0- Chấn động (não do tai nạn)</t>
+  </si>
+  <si>
+    <t>K07.9- Bất thường hàm mặt không xác định (Vết thương phần mềm, tụ máu vùng</t>
+  </si>
+  <si>
+    <t>hàm mặt)</t>
+  </si>
+  <si>
+    <t>- Phương pháp điều trị:</t>
+  </si>
+  <si>
+    <t>Kháng sinh, giảm nề, chống viêm.</t>
+  </si>
+  <si>
+    <t>- Ghi chú:</t>
+  </si>
+  <si>
+    <t>Cho bệnh nhân nghi thêm từ ngày 07/10/2022 đến hết ngày 10/10/2022</t>
+  </si>
+  <si>
+    <t>Khám lại ngay khi có dấu hiệu bất thường</t>
+  </si>
+  <si>
+    <t>Ngày 06 tháng 10 năm 2022</t>
+  </si>
+  <si>
+    <t>Thủ trưởng đơn, vị</t>
+  </si>
+  <si>
+    <t>Trưởng khoa</t>
+  </si>
+  <si>
+    <t>Ký tên đóng dâu)</t>
+  </si>
+  <si>
+    <t>BS.CKI: Nềng Đức Thạch</t>
+  </si>
+  <si>
+    <t>B8: CKI: Nguyễn Văn Tạ</t>
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>[(361, 128), (788, 120), (789, 144), (361, 152)]</t>
+  </si>
+  <si>
+    <t>[(134, 121), (330, 121), (330, 141), (134, 141)]</t>
+  </si>
+  <si>
+    <t>[(109, 146), (353, 147), (353, 166), (109, 164)]</t>
+  </si>
+  <si>
+    <t>[(692, 151), (874, 147), (875, 166), (693, 170)]</t>
+  </si>
+  <si>
+    <t>[(422, 153), (625, 151), (625, 172), (422, 173)]</t>
+  </si>
+  <si>
+    <t>[(151, 168), (312, 172), (311, 193), (150, 190)]</t>
+  </si>
+  <si>
+    <t>[(691, 175), (864, 172), (864, 191), (692, 194)]</t>
+  </si>
+  <si>
+    <t>[(425, 202), (577, 202), (577, 225), (425, 225)]</t>
+  </si>
+  <si>
+    <t>[(827, 228), (853, 228), (853, 247), (827, 247)]</t>
+  </si>
+  <si>
+    <t>[(108, 226), (428, 229), (427, 251), (108, 248)]</t>
+  </si>
+  <si>
+    <t>[(671, 229), (767, 227), (767, 248), (671, 250)]</t>
+  </si>
+  <si>
+    <t>[(107, 254), (207, 254), (207, 273), (107, 273)]</t>
+  </si>
+  <si>
+    <t>[(207, 253), (271, 256), (270, 276), (206, 272)]</t>
+  </si>
+  <si>
+    <t>[(473, 253), (668, 256), (668, 278), (473, 275)]</t>
+  </si>
+  <si>
+    <t>[(107, 276), (339, 276), (339, 297), (107, 297)]</t>
+  </si>
+  <si>
+    <t>[(410, 279), (689, 279), (689, 298), (410, 298)]</t>
+  </si>
+  <si>
+    <t>[(107, 302), (184, 302), (184, 322), (107, 322)]</t>
+  </si>
+  <si>
+    <t>[(210, 302), (501, 304), (501, 324), (210, 322)]</t>
+  </si>
+  <si>
+    <t>[(107, 325), (220, 328), (220, 347), (106, 345)]</t>
+  </si>
+  <si>
+    <t>[(275, 327), (594, 329), (593, 350), (275, 348)]</t>
+  </si>
+  <si>
+    <t>[(107, 351), (211, 351), (211, 370), (107, 370)]</t>
+  </si>
+  <si>
+    <t>[(276, 352), (593, 351), (594, 373), (276, 374)]</t>
+  </si>
+  <si>
+    <t>[(107, 376), (207, 376), (207, 395), (107, 395)]</t>
+  </si>
+  <si>
+    <t>[(279, 373), (535, 375), (535, 397), (279, 395)]</t>
+  </si>
+  <si>
+    <t>[(279, 398), (898, 401), (898, 422), (279, 419)]</t>
+  </si>
+  <si>
+    <t>[(94, 424), (167, 426), (167, 445), (93, 443)]</t>
+  </si>
+  <si>
+    <t>[(105, 448), (290, 446), (290, 468), (106, 470)]</t>
+  </si>
+  <si>
+    <t>[(291, 446), (560, 449), (560, 470), (291, 467)]</t>
+  </si>
+  <si>
+    <t>[(106, 472), (185, 472), (185, 492), (106, 492)]</t>
+  </si>
+  <si>
+    <t>[(210, 471), (747, 474), (746, 495), (210, 491)]</t>
+  </si>
+  <si>
+    <t>[(210, 494), (528, 496), (528, 519), (210, 516)]</t>
+  </si>
+  <si>
+    <t>[(140, 521), (352, 521), (352, 543), (140, 543)]</t>
+  </si>
+  <si>
+    <t>[(642, 520), (861, 524), (860, 546), (642, 542)]</t>
+  </si>
+  <si>
+    <t>[(171, 541), (323, 541), (323, 561), (171, 561)]</t>
+  </si>
+  <si>
+    <t>[(698, 541), (811, 547), (810, 568), (697, 562)]</t>
+  </si>
+  <si>
+    <t>[(181, 560), (320, 560), (320, 576), (181, 576)]</t>
+  </si>
+  <si>
+    <t>[(650, 652), (870, 661), (869, 692), (649, 683)]</t>
+  </si>
+  <si>
+    <t>[(198, 677), (408, 675), (408, 706), (198, 708)]</t>
   </si>
 </sst>
 </file>
@@ -494,13 +620,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,810 +645,996 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>413</v>
+        <v>361</v>
       </c>
       <c r="C2">
-        <v>451</v>
+        <v>789</v>
       </c>
       <c r="D2">
-        <v>237</v>
+        <v>120</v>
       </c>
       <c r="E2">
-        <v>252</v>
+        <v>152</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>366</v>
+        <v>134</v>
       </c>
       <c r="C3">
-        <v>502</v>
+        <v>330</v>
       </c>
       <c r="D3">
-        <v>245</v>
+        <v>121</v>
       </c>
       <c r="E3">
-        <v>273</v>
+        <v>141</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C4">
-        <v>141</v>
+        <v>353</v>
       </c>
       <c r="D4">
-        <v>264</v>
+        <v>146</v>
       </c>
       <c r="E4">
-        <v>278</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>72</v>
+        <v>692</v>
       </c>
       <c r="C5">
-        <v>165</v>
+        <v>875</v>
       </c>
       <c r="D5">
-        <v>274</v>
+        <v>147</v>
       </c>
       <c r="E5">
-        <v>296</v>
+        <v>170</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>422</v>
       </c>
       <c r="C6">
-        <v>435</v>
+        <v>625</v>
       </c>
       <c r="D6">
-        <v>278</v>
+        <v>151</v>
       </c>
       <c r="E6">
-        <v>300</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>445</v>
+        <v>150</v>
       </c>
       <c r="C7">
-        <v>514</v>
+        <v>312</v>
       </c>
       <c r="D7">
-        <v>281</v>
+        <v>168</v>
       </c>
       <c r="E7">
-        <v>300</v>
+        <v>193</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>47</v>
+        <v>691</v>
       </c>
       <c r="C8">
-        <v>188</v>
+        <v>864</v>
       </c>
       <c r="D8">
-        <v>289</v>
+        <v>172</v>
       </c>
       <c r="E8">
-        <v>315</v>
+        <v>194</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>243</v>
+        <v>425</v>
       </c>
       <c r="C9">
-        <v>381</v>
+        <v>577</v>
       </c>
       <c r="D9">
-        <v>295</v>
+        <v>202</v>
       </c>
       <c r="E9">
-        <v>315</v>
+        <v>225</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>469</v>
+        <v>827</v>
       </c>
       <c r="C10">
-        <v>514</v>
+        <v>853</v>
       </c>
       <c r="D10">
-        <v>297</v>
+        <v>228</v>
       </c>
       <c r="E10">
-        <v>310</v>
+        <v>247</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="C11">
-        <v>156</v>
+        <v>428</v>
       </c>
       <c r="D11">
-        <v>306</v>
+        <v>226</v>
       </c>
       <c r="E11">
-        <v>321</v>
+        <v>251</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>412</v>
+        <v>671</v>
       </c>
       <c r="C12">
-        <v>515</v>
+        <v>767</v>
       </c>
       <c r="D12">
-        <v>306</v>
+        <v>227</v>
       </c>
       <c r="E12">
-        <v>325</v>
+        <v>250</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C13">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="D13">
-        <v>317</v>
+        <v>254</v>
       </c>
       <c r="E13">
-        <v>333</v>
+        <v>273</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>53</v>
+        <v>206</v>
       </c>
       <c r="C14">
-        <v>185</v>
+        <v>271</v>
       </c>
       <c r="D14">
-        <v>331</v>
+        <v>253</v>
       </c>
       <c r="E14">
-        <v>350</v>
+        <v>276</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>266</v>
+        <v>473</v>
       </c>
       <c r="C15">
-        <v>363</v>
+        <v>668</v>
       </c>
       <c r="D15">
-        <v>368</v>
+        <v>253</v>
       </c>
       <c r="E15">
-        <v>385</v>
+        <v>278</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C16">
-        <v>272</v>
+        <v>339</v>
       </c>
       <c r="D16">
-        <v>394</v>
+        <v>276</v>
       </c>
       <c r="E16">
-        <v>412</v>
+        <v>297</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>381</v>
+        <v>410</v>
       </c>
       <c r="C17">
-        <v>507</v>
+        <v>689</v>
       </c>
       <c r="D17">
-        <v>396</v>
+        <v>279</v>
       </c>
       <c r="E17">
-        <v>413</v>
+        <v>298</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C18">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="D18">
-        <v>420</v>
+        <v>302</v>
       </c>
       <c r="E18">
-        <v>440</v>
+        <v>322</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>261</v>
+        <v>210</v>
       </c>
       <c r="C19">
-        <v>413</v>
+        <v>501</v>
       </c>
       <c r="D19">
-        <v>421</v>
+        <v>302</v>
       </c>
       <c r="E19">
-        <v>440</v>
+        <v>324</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="C20">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D20">
-        <v>440</v>
+        <v>325</v>
       </c>
       <c r="E20">
-        <v>457</v>
+        <v>347</v>
       </c>
       <c r="F20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="C21">
-        <v>488</v>
+        <v>594</v>
       </c>
       <c r="D21">
-        <v>440</v>
+        <v>327</v>
       </c>
       <c r="E21">
-        <v>458</v>
+        <v>350</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="C22">
-        <v>458</v>
+        <v>211</v>
       </c>
       <c r="D22">
-        <v>470</v>
+        <v>351</v>
       </c>
       <c r="E22">
-        <v>489</v>
+        <v>370</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>72</v>
+        <v>276</v>
       </c>
       <c r="C23">
+        <v>594</v>
+      </c>
+      <c r="D23">
+        <v>351</v>
+      </c>
+      <c r="E23">
         <v>374</v>
       </c>
-      <c r="D23">
-        <v>494</v>
-      </c>
-      <c r="E23">
-        <v>512</v>
-      </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="C24">
-        <v>374</v>
+        <v>207</v>
       </c>
       <c r="D24">
-        <v>516</v>
+        <v>376</v>
       </c>
       <c r="E24">
-        <v>534</v>
+        <v>395</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>72</v>
+        <v>279</v>
       </c>
       <c r="C25">
-        <v>141</v>
+        <v>535</v>
       </c>
       <c r="D25">
-        <v>517</v>
+        <v>373</v>
       </c>
       <c r="E25">
-        <v>534</v>
+        <v>397</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>72</v>
+        <v>279</v>
       </c>
       <c r="C26">
-        <v>401</v>
+        <v>898</v>
       </c>
       <c r="D26">
-        <v>537</v>
+        <v>398</v>
       </c>
       <c r="E26">
-        <v>562</v>
+        <v>422</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>383</v>
+        <v>93</v>
       </c>
       <c r="C27">
-        <v>507</v>
+        <v>167</v>
       </c>
       <c r="D27">
-        <v>559</v>
+        <v>424</v>
       </c>
       <c r="E27">
-        <v>580</v>
+        <v>445</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="C28">
-        <v>385</v>
+        <v>290</v>
       </c>
       <c r="D28">
-        <v>562</v>
+        <v>446</v>
       </c>
       <c r="E28">
-        <v>583</v>
+        <v>470</v>
       </c>
       <c r="F28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
+        <v>291</v>
+      </c>
+      <c r="C29">
+        <v>560</v>
+      </c>
+      <c r="D29">
+        <v>446</v>
+      </c>
+      <c r="E29">
+        <v>470</v>
+      </c>
+      <c r="F29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" t="s">
         <v>72</v>
       </c>
-      <c r="C29">
-        <v>234</v>
-      </c>
-      <c r="D29">
-        <v>578</v>
-      </c>
-      <c r="E29">
-        <v>598</v>
-      </c>
-      <c r="F29" t="s">
-        <v>33</v>
-      </c>
-      <c r="G29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C30">
-        <v>120</v>
+        <v>185</v>
       </c>
       <c r="D30">
-        <v>600</v>
+        <v>472</v>
       </c>
       <c r="E30">
-        <v>618</v>
+        <v>492</v>
       </c>
       <c r="F30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>330</v>
+        <v>210</v>
       </c>
       <c r="C31">
-        <v>452</v>
+        <v>747</v>
       </c>
       <c r="D31">
-        <v>623</v>
+        <v>471</v>
       </c>
       <c r="E31">
-        <v>642</v>
+        <v>495</v>
       </c>
       <c r="F31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>119</v>
+        <v>210</v>
       </c>
       <c r="C32">
-        <v>246</v>
+        <v>528</v>
       </c>
       <c r="D32">
-        <v>626</v>
+        <v>494</v>
       </c>
       <c r="E32">
-        <v>645</v>
+        <v>519</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H32" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>333</v>
+        <v>140</v>
       </c>
       <c r="C33">
-        <v>431</v>
+        <v>352</v>
       </c>
       <c r="D33">
-        <v>641</v>
+        <v>521</v>
       </c>
       <c r="E33">
-        <v>658</v>
+        <v>543</v>
       </c>
       <c r="F33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G33" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>119</v>
+        <v>642</v>
       </c>
       <c r="C34">
-        <v>245</v>
+        <v>861</v>
       </c>
       <c r="D34">
-        <v>642</v>
+        <v>520</v>
       </c>
       <c r="E34">
-        <v>665</v>
+        <v>546</v>
       </c>
       <c r="F34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>360</v>
+        <v>171</v>
       </c>
       <c r="C35">
-        <v>417</v>
+        <v>323</v>
       </c>
       <c r="D35">
-        <v>721</v>
+        <v>541</v>
       </c>
       <c r="E35">
-        <v>739</v>
+        <v>561</v>
       </c>
       <c r="F35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>44</v>
+      </c>
+      <c r="H35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>103</v>
+        <v>697</v>
       </c>
       <c r="C36">
-        <v>261</v>
+        <v>811</v>
       </c>
       <c r="D36">
-        <v>754</v>
+        <v>541</v>
       </c>
       <c r="E36">
-        <v>777</v>
+        <v>568</v>
       </c>
       <c r="F36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G36" t="s">
-        <v>40</v>
+        <v>44</v>
+      </c>
+      <c r="H36" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>181</v>
+      </c>
+      <c r="C37">
+        <v>320</v>
+      </c>
+      <c r="D37">
+        <v>560</v>
+      </c>
+      <c r="E37">
+        <v>576</v>
+      </c>
+      <c r="F37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>649</v>
+      </c>
+      <c r="C38">
+        <v>870</v>
+      </c>
+      <c r="D38">
+        <v>652</v>
+      </c>
+      <c r="E38">
+        <v>692</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>198</v>
+      </c>
+      <c r="C39">
+        <v>408</v>
+      </c>
+      <c r="D39">
+        <v>675</v>
+      </c>
+      <c r="E39">
+        <v>708</v>
+      </c>
+      <c r="F39" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>